<commit_message>
[DANIEL] Inclusion interfaz activacion de tareas
</commit_message>
<xml_diff>
--- a/Jornada de trabajo.xlsx
+++ b/Jornada de trabajo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>Semana 1 Julio</t>
   </si>
@@ -58,14 +58,32 @@
     <t>Horas;</t>
   </si>
   <si>
-    <t>16/20</t>
+    <t>21/20</t>
+  </si>
+  <si>
+    <t>Semana 8 Julio</t>
+  </si>
+  <si>
+    <t>Trabajo realizado:</t>
+  </si>
+  <si>
+    <t>Sabado</t>
+  </si>
+  <si>
+    <t>Correcion negligencias previas</t>
+  </si>
+  <si>
+    <t>Correccion errores</t>
+  </si>
+  <si>
+    <t>Creacion Inicializadores Tareas Simples</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,8 +99,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -101,8 +125,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -110,17 +158,128 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,192 +560,864 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:N21"/>
+  <dimension ref="B3:X42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="Q19" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="2.6640625" customWidth="1"/>
+    <col min="16" max="16" width="3.44140625" customWidth="1"/>
+    <col min="18" max="20" width="27.44140625" customWidth="1"/>
+    <col min="21" max="21" width="32.6640625" customWidth="1"/>
+    <col min="22" max="24" width="27.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
+    <row r="3" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B4" s="19" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="D6" t="s">
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="21"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="5"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B6" s="3"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="L6" s="4"/>
+      <c r="M6" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="1">
+      <c r="N6" s="4"/>
+      <c r="P6" s="5"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B7" s="3"/>
+      <c r="C7" s="11">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="11">
         <v>0.375</v>
       </c>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="1">
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="P7" s="5"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B8" s="3"/>
+      <c r="C8" s="11">
         <v>0.375</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="11">
         <v>0.41666666666666702</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="2"/>
-      <c r="M8" t="s">
+      <c r="E8" s="14"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="1">
+      <c r="P8" s="5"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B9" s="3"/>
+      <c r="C9" s="11">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="11">
         <v>0.45833333333333298</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="1">
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="5"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B10" s="3"/>
+      <c r="C10" s="11">
         <v>0.45833333333333298</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="11">
         <v>0.5</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="1">
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="5"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B11" s="3"/>
+      <c r="C11" s="11">
         <v>0.5</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="11">
         <v>0.54166666666666696</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="1">
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="5"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B12" s="3"/>
+      <c r="C12" s="11">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="11">
         <v>0.58333333333333504</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="1">
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="5"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B13" s="3"/>
+      <c r="C13" s="11">
         <v>0.58333333333333304</v>
       </c>
-      <c r="C13" s="1">
+      <c r="D13" s="11">
         <v>0.625000000000002</v>
       </c>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="1">
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="5"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B14" s="3"/>
+      <c r="C14" s="11">
         <v>0.625</v>
       </c>
-      <c r="C14" s="1">
+      <c r="D14" s="11">
         <v>0.66666666666666896</v>
       </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="1">
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="5"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B15" s="3"/>
+      <c r="C15" s="11">
         <v>0.66666666666666696</v>
       </c>
-      <c r="C15" s="1">
+      <c r="D15" s="11">
         <v>0.70833333333333603</v>
       </c>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="1">
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="5"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B16" s="3"/>
+      <c r="C16" s="11">
         <v>0.70833333333333304</v>
       </c>
-      <c r="C16" s="1">
+      <c r="D16" s="11">
         <v>0.750000000000003</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="1">
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="5"/>
+    </row>
+    <row r="17" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B17" s="3"/>
+      <c r="C17" s="11">
         <v>0.75</v>
       </c>
-      <c r="C17" s="1">
+      <c r="D17" s="11">
         <v>0.79166666666666996</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="1">
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="5"/>
+    </row>
+    <row r="18" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B18" s="3"/>
+      <c r="C18" s="11">
         <v>0.79166666666666696</v>
       </c>
-      <c r="C18" s="1">
+      <c r="D18" s="11">
         <v>0.83333333333333703</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" s="1">
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="5"/>
+    </row>
+    <row r="19" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B19" s="3"/>
+      <c r="C19" s="11">
         <v>0.83333333333333304</v>
       </c>
-      <c r="C19" s="1">
+      <c r="D19" s="11">
         <v>0.875000000000004</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B20" s="1">
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="5"/>
+    </row>
+    <row r="20" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B20" s="3"/>
+      <c r="C20" s="11">
         <v>0.875</v>
       </c>
-      <c r="C20" s="1">
+      <c r="D20" s="11">
         <v>0.91666666666667096</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B21" s="1">
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="5"/>
+    </row>
+    <row r="21" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B21" s="3"/>
+      <c r="C21" s="11">
         <v>0.91666666666666696</v>
       </c>
-      <c r="C21" s="1">
+      <c r="D21" s="11">
         <v>0.95833333333333803</v>
       </c>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="5"/>
+    </row>
+    <row r="22" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="7"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="9"/>
+    </row>
+    <row r="23" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B24" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="20"/>
+      <c r="O24" s="20"/>
+      <c r="P24" s="21"/>
+    </row>
+    <row r="25" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B25" s="3"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="5"/>
+    </row>
+    <row r="26" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B26" s="3"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K26" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="L26" s="4"/>
+      <c r="M26" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N26" s="4"/>
+      <c r="P26" s="5"/>
+      <c r="R26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B27" s="3"/>
+      <c r="C27" s="11">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D27" s="11">
+        <v>0.375</v>
+      </c>
+      <c r="E27" s="12"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="P27" s="5"/>
+    </row>
+    <row r="28" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B28" s="3"/>
+      <c r="C28" s="11">
+        <v>0.375</v>
+      </c>
+      <c r="D28" s="11">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="E28" s="14"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N28" s="4"/>
+      <c r="P28" s="5"/>
+      <c r="R28" t="s">
+        <v>1</v>
+      </c>
+      <c r="S28" t="s">
+        <v>2</v>
+      </c>
+      <c r="T28" t="s">
+        <v>3</v>
+      </c>
+      <c r="U28" t="s">
+        <v>4</v>
+      </c>
+      <c r="V28" t="s">
+        <v>5</v>
+      </c>
+      <c r="W28" t="s">
+        <v>15</v>
+      </c>
+      <c r="X28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B29" s="3"/>
+      <c r="C29" s="11">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="D29" s="11">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="E29" s="14"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="5"/>
+      <c r="R29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B30" s="3"/>
+      <c r="C30" s="11">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="D30" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="E30" s="14"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="5"/>
+      <c r="R30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B31" s="3"/>
+      <c r="C31" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="D31" s="11">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="E31" s="14"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="5"/>
+      <c r="R31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B32" s="3"/>
+      <c r="C32" s="11">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="D32" s="11">
+        <v>0.58333333333333504</v>
+      </c>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="5"/>
+      <c r="R32" s="17"/>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B33" s="3"/>
+      <c r="C33" s="11">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="D33" s="11">
+        <v>0.625000000000002</v>
+      </c>
+      <c r="E33" s="12"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="5"/>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B34" s="3"/>
+      <c r="C34" s="11">
+        <v>0.625</v>
+      </c>
+      <c r="D34" s="11">
+        <v>0.66666666666666896</v>
+      </c>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="5"/>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B35" s="3"/>
+      <c r="C35" s="11">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="D35" s="11">
+        <v>0.70833333333333603</v>
+      </c>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="5"/>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B36" s="3"/>
+      <c r="C36" s="11">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="D36" s="11">
+        <v>0.750000000000003</v>
+      </c>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="5"/>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B37" s="3"/>
+      <c r="C37" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="D37" s="11">
+        <v>0.79166666666666996</v>
+      </c>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="12"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="5"/>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B38" s="3"/>
+      <c r="C38" s="11">
+        <v>0.79166666666666696</v>
+      </c>
+      <c r="D38" s="11">
+        <v>0.83333333333333703</v>
+      </c>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="5"/>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B39" s="3"/>
+      <c r="C39" s="11">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="D39" s="11">
+        <v>0.875000000000004</v>
+      </c>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="12"/>
+      <c r="K39" s="12"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="5"/>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B40" s="3"/>
+      <c r="C40" s="11">
+        <v>0.875</v>
+      </c>
+      <c r="D40" s="11">
+        <v>0.91666666666667096</v>
+      </c>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="12"/>
+      <c r="K40" s="12"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4"/>
+      <c r="P40" s="5"/>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B41" s="3"/>
+      <c r="C41" s="11">
+        <v>0.91666666666666696</v>
+      </c>
+      <c r="D41" s="11">
+        <v>0.95833333333333803</v>
+      </c>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="12"/>
+      <c r="K41" s="12"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="5"/>
+    </row>
+    <row r="42" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="7"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="9"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B4:P4"/>
+    <mergeCell ref="B24:P24"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -603,13 +1434,13 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="5" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C5" s="2"/>
+      <c r="C5" s="1"/>
       <c r="D5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C6" s="3"/>
+      <c r="C6" s="2"/>
       <c r="D6" t="s">
         <v>9</v>
       </c>

</xml_diff>